<commit_message>
add unpacking function, check columns type
</commit_message>
<xml_diff>
--- a/form.xlsx
+++ b/form.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>в/ч</t>
   </si>
@@ -31,13 +31,43 @@
   </si>
   <si>
     <t>Сотрудники СиС(ФИО)</t>
+  </si>
+  <si>
+    <t>Номер предписания</t>
+  </si>
+  <si>
+    <t>дата</t>
+  </si>
+  <si>
+    <t>Ткаченко Ярослав Александрович</t>
+  </si>
+  <si>
+    <t>инвентаризация</t>
+  </si>
+  <si>
+    <t>461000, Оренбургская обл., п. Колтубановка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2173 ЦАС  (1 разряда) </t>
+  </si>
+  <si>
+    <t>Техник ТСО</t>
+  </si>
+  <si>
+    <t>Полевков Александр Николаевич</t>
+  </si>
+  <si>
+    <t>Ткаченко Александр Васильевич</t>
+  </si>
+  <si>
+    <t>Инженер ТСО</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,6 +75,20 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -82,12 +126,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -389,128 +461,204 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>615</v>
+      </c>
+      <c r="B2" s="9">
+        <v>41330</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>616</v>
+      </c>
+      <c r="B3" s="9">
+        <v>41330</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>617</v>
+      </c>
+      <c r="B4" s="9">
+        <v>41330</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>